<commit_message>
Deploying to gh-pages from @ pimborman/nixie-clock@de780db2857f2b30e7a47e9d26594c67cc7b3d3c 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/nixie-bom.xlsx
+++ b/BoM/Costs/nixie-bom.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="218">
   <si>
     <t>Row</t>
   </si>
@@ -443,7 +443,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>R1 R2 R3 R4</t>
+    <t>R1</t>
   </si>
   <si>
     <t>R_Axial_DIN0207_L6.3mm_D2.5mm_P7.62mm_Horizontal</t>
@@ -452,13 +452,19 @@
     <t>18</t>
   </si>
   <si>
-    <t>R15 R17 R22</t>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>R3 R15 R17 R22</t>
   </si>
   <si>
     <t>4.7k</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>R16 R18 R19 R20 R21 R23</t>
@@ -467,7 +473,7 @@
     <t>10k</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>R5 R6 R7 R8 R9 R10 R11 R12 R13 R14</t>
@@ -476,7 +482,16 @@
     <t>15k</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>800k</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
   <si>
     <t>R_Potentiometer_Trim</t>
@@ -491,7 +506,7 @@
     <t>Potentiometer_Bourns_3306P_Vertical</t>
   </si>
   <si>
-    <t>22</t>
+    <t>24</t>
   </si>
   <si>
     <t>RotaryEncoder_Switch</t>
@@ -503,7 +518,7 @@
     <t>PEC11H4020FS0016</t>
   </si>
   <si>
-    <t>23</t>
+    <t>25</t>
   </si>
   <si>
     <t>4504</t>
@@ -518,7 +533,7 @@
     <t>http://www.ti.com/lit/ds/symlink/cd4504b.pdf</t>
   </si>
   <si>
-    <t>24</t>
+    <t>26</t>
   </si>
   <si>
     <t>ATmega328P-P</t>
@@ -533,7 +548,7 @@
     <t>http://ww1.microchip.com/downloads/en/DeviceDoc/ATmega328_P%20AVR%20MCU%20with%20picoPower%20Technology%20Data%20Sheet%2040001984A.pdf</t>
   </si>
   <si>
-    <t>25</t>
+    <t>27</t>
   </si>
   <si>
     <t>DS3231MZ</t>
@@ -548,7 +563,7 @@
     <t>http://datasheets.maximintegrated.com/en/ds/DS3231M.pdf</t>
   </si>
   <si>
-    <t>26</t>
+    <t>28</t>
   </si>
   <si>
     <t>HV5222PG-G</t>
@@ -578,7 +593,7 @@
     <t>https://www.arrow.com/en/products/hv5222pg-g/microchip-technology</t>
   </si>
   <si>
-    <t>27</t>
+    <t>29</t>
   </si>
   <si>
     <t>LM7805_TO220</t>
@@ -590,7 +605,7 @@
     <t>https://www.onsemi.cn/PowerSolutions/document/MC7800-D.PDF</t>
   </si>
   <si>
-    <t>28</t>
+    <t>30</t>
   </si>
   <si>
     <t>MC34063AP</t>
@@ -623,7 +638,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>v1.0</t>
+    <t>v1.1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -743,7 +758,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-13 09:48:50</t>
+    <t>2024-10-13 16:32:31</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1521,7 +1536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1552,7 +1567,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1572,55 +1587,55 @@
     </row>
     <row r="2" spans="1:18">
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F2" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="C4" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="C5" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1628,13 +1643,13 @@
     </row>
     <row r="6" spans="1:18">
       <c r="C6" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F6" s="3">
         <v>66</v>
@@ -2612,7 +2627,7 @@
         <v>97</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>23</v>
@@ -2662,13 +2677,13 @@
         <v>99</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>97</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>23</v>
@@ -2706,7 +2721,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>19</v>
@@ -2715,16 +2730,16 @@
         <v>95</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>97</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>23</v>
@@ -2762,7 +2777,7 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>19</v>
@@ -2771,16 +2786,16 @@
         <v>95</v>
       </c>
       <c r="D28" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>97</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>23</v>
@@ -2818,25 +2833,25 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>23</v>
@@ -2874,22 +2889,22 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>18</v>
@@ -2930,22 +2945,22 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>18</v>
@@ -2953,55 +2968,55 @@
       <c r="H31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R31" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="45" customHeight="1">
-      <c r="A32" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>18</v>
@@ -3009,8 +3024,8 @@
       <c r="H32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="10" t="s">
-        <v>125</v>
+      <c r="I32" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>19</v>
@@ -3042,22 +3057,22 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>18</v>
@@ -3066,7 +3081,7 @@
         <v>23</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>19</v>
@@ -3096,33 +3111,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="30" customHeight="1">
+    <row r="34" spans="1:18" ht="45" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J34" s="9" t="s">
         <v>19</v>
@@ -3130,46 +3145,46 @@
       <c r="K34" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="N34" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="O34" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q34" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R34" s="12" t="s">
-        <v>140</v>
+      <c r="L34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R34" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="5" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>18</v>
@@ -3178,7 +3193,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>19</v>
@@ -3208,59 +3223,171 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I36" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="P36" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q36" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="R36" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="J36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R36" s="9" t="s">
+      <c r="J37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R38" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3276,7 +3403,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
@@ -3299,7 +3426,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3308,13 +3435,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -3322,13 +3449,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3337,38 +3464,38 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="H4" s="16">
-        <f>SUM(H10:H37)</f>
+        <f>SUM(H10:H39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3392,16 +3519,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3412,7 +3539,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>22</v>
@@ -3434,7 +3561,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>29</v>
@@ -3456,7 +3583,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>33</v>
@@ -3478,7 +3605,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>33</v>
@@ -3500,7 +3627,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>42</v>
@@ -3522,7 +3649,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>46</v>
@@ -3544,7 +3671,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>50</v>
@@ -3569,7 +3696,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>58</v>
@@ -3594,7 +3721,7 @@
         <v>61</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>62</v>
@@ -3616,7 +3743,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>66</v>
@@ -3638,7 +3765,7 @@
         <v>68</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>70</v>
@@ -3660,7 +3787,7 @@
         <v>45</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>74</v>
@@ -3720,7 +3847,7 @@
         <v>84</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>86</v>
@@ -3745,7 +3872,7 @@
         <v>91</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>92</v>
@@ -3770,14 +3897,14 @@
         <v>95</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>97</v>
       </c>
       <c r="F26" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H26" s="20">
         <f>IF(AND(ISNUMBER(F26),ISNUMBER(G26)),F26*G26,"")</f>
@@ -3789,17 +3916,17 @@
         <v>99</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H27" s="20">
         <f>IF(AND(ISNUMBER(F27),ISNUMBER(G27)),F27*G27,"")</f>
@@ -3808,20 +3935,20 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>103</v>
-      </c>
       <c r="C28" s="19" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>97</v>
       </c>
       <c r="F28" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="H28" s="20">
         <f>IF(AND(ISNUMBER(F28),ISNUMBER(G28)),F28*G28,"")</f>
@@ -3830,20 +3957,20 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>106</v>
-      </c>
       <c r="C29" s="19" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>97</v>
       </c>
       <c r="F29" s="19">
-        <f>CEILING(BoardQty*10,1)</f>
-        <v>10</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="H29" s="20">
         <f>IF(AND(ISNUMBER(F29),ISNUMBER(G29)),F29*G29,"")</f>
@@ -3852,38 +3979,38 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F30" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*10,1)</f>
+        <v>10</v>
       </c>
       <c r="H30" s="20">
         <f>IF(AND(ISNUMBER(F30),ISNUMBER(G30)),F30*G30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" customHeight="1">
+    <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="F31" s="19">
         <f>BoardQty*1</f>
@@ -3894,21 +4021,18 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" customHeight="1">
+    <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F32" s="19">
         <f>BoardQty*1</f>
@@ -3919,21 +4043,18 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45" customHeight="1">
+    <row r="33" spans="1:8" ht="30" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F33" s="19">
         <f>BoardQty*1</f>
@@ -3944,21 +4065,21 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F34" s="19">
         <f>BoardQty*1</f>
@@ -3969,25 +4090,25 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" customHeight="1">
+    <row r="35" spans="1:8" ht="45" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F35" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H35" s="20">
         <f>IF(AND(ISNUMBER(F35),ISNUMBER(G35)),F35*G35,"")</f>
@@ -3996,19 +4117,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F36" s="19">
         <f>BoardQty*1</f>
@@ -4021,40 +4142,90 @@
     </row>
     <row r="37" spans="1:8" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F37" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="H37" s="20">
         <f>IF(AND(ISNUMBER(F37),ISNUMBER(G37)),F37*G37,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="21" t="s">
+    <row r="38" spans="1:8">
+      <c r="A38" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="D38" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="20">
+        <f>IF(AND(ISNUMBER(F38),ISNUMBER(G38)),F38*G38,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" customHeight="1">
+      <c r="A39" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="23" t="s">
-        <v>197</v>
+      <c r="D39" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F39" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="20">
+        <f>IF(AND(ISNUMBER(F39),ISNUMBER(G39)),F39*G39,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="23" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4202,17 +4373,27 @@
       <formula>AND(ISBLANK(E37),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F38">
+    <cfRule type="expression" dxfId="0" priority="29">
+      <formula>AND(ISBLANK(E38),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="expression" dxfId="0" priority="30">
+      <formula>AND(ISBLANK(E39),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E16" r:id="rId1"/>
     <hyperlink ref="E17" r:id="rId2"/>
     <hyperlink ref="E24" r:id="rId3"/>
     <hyperlink ref="E25" r:id="rId4"/>
-    <hyperlink ref="E32" r:id="rId5"/>
-    <hyperlink ref="E33" r:id="rId6"/>
-    <hyperlink ref="E34" r:id="rId7"/>
-    <hyperlink ref="E35" r:id="rId8"/>
-    <hyperlink ref="E36" r:id="rId9"/>
-    <hyperlink ref="E37" r:id="rId10"/>
+    <hyperlink ref="E34" r:id="rId5"/>
+    <hyperlink ref="E35" r:id="rId6"/>
+    <hyperlink ref="E36" r:id="rId7"/>
+    <hyperlink ref="E37" r:id="rId8"/>
+    <hyperlink ref="E38" r:id="rId9"/>
+    <hyperlink ref="E39" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId11"/>
@@ -4233,77 +4414,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>